<commit_message>
Minor fixes and renaming
</commit_message>
<xml_diff>
--- a/assets/spreadsheets/ojt-001/ojt-001-TIME_SHEET_SUMMARY_.xlsx
+++ b/assets/spreadsheets/ojt-001/ojt-001-TIME_SHEET_SUMMARY_.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>WEEKLY TIME SHEET SUMMARY</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>2026-02-06</t>
+  </si>
+  <si>
+    <t>2026-02-09</t>
+  </si>
+  <si>
+    <t>2026-02-10</t>
+  </si>
+  <si>
+    <t>2026-02-11</t>
   </si>
 </sst>
 </file>
@@ -499,10 +508,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:D13"/>
+      <selection activeCell="A1" sqref="A1:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -682,6 +691,48 @@
         <v>8</v>
       </c>
     </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:D2"/>

</xml_diff>

<commit_message>
Fixed time sheet total hours computation and display
</commit_message>
<xml_diff>
--- a/assets/spreadsheets/ojt-001/ojt-001-TIME_SHEET_SUMMARY_.xlsx
+++ b/assets/spreadsheets/ojt-001/ojt-001-TIME_SHEET_SUMMARY_.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>WEEKLY TIME SHEET SUMMARY</t>
   </si>
@@ -32,6 +32,9 @@
     <t>TOTAL HOURS</t>
   </si>
   <si>
+    <t>DISPLAY HOURS</t>
+  </si>
+  <si>
     <t>2026-01-26</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
     <t>4:00 PM</t>
   </si>
   <si>
+    <t>8 hours</t>
+  </si>
+  <si>
     <t>2026-01-27</t>
   </si>
   <si>
@@ -65,6 +71,9 @@
     <t>1:00 PM</t>
   </si>
   <si>
+    <t>5 hours</t>
+  </si>
+  <si>
     <t>2026-02-05</t>
   </si>
   <si>
@@ -78,6 +87,15 @@
   </si>
   <si>
     <t>2026-02-11</t>
+  </si>
+  <si>
+    <t>2026-02-12</t>
+  </si>
+  <si>
+    <t>7:37 AM</t>
+  </si>
+  <si>
+    <t>8 hours and 23 minutes</t>
   </si>
 </sst>
 </file>
@@ -137,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -160,16 +178,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -508,10 +541,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:D16"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A10">
+      <selection activeCell="A1" sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -520,22 +553,24 @@
     <col min="2" max="2" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="15.139" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="17.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="14.85546875" customWidth="true" style="0"/>
+    <col min="5" max="5" width="18.140625" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" customHeight="1" ht="21">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" customHeight="1" ht="15">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" customHeight="1" ht="15.75">
       <c r="A3" s="1" t="s">
@@ -550,192 +585,251 @@
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
         <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
         <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
         <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2">
         <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2">
         <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
         <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2">
         <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2">
         <v>5</v>
       </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" s="2">
         <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D13" s="2">
         <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="2">
         <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" s="2">
         <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" s="2">
         <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2">
+        <v>8.38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="A1:E2"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed time sheet summary total hours display
</commit_message>
<xml_diff>
--- a/assets/spreadsheets/ojt-001/ojt-001-TIME_SHEET_SUMMARY_.xlsx
+++ b/assets/spreadsheets/ojt-001/ojt-001-TIME_SHEET_SUMMARY_.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>WEEKLY TIME SHEET SUMMARY</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>2026-02-13</t>
-  </si>
-  <si>
-    <t>8 hours and 0 minutes</t>
   </si>
 </sst>
 </file>
@@ -161,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -184,31 +181,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -550,7 +532,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A10">
-      <selection activeCell="A1" sqref="A1:D18"/>
+      <selection activeCell="A1" sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -559,24 +541,24 @@
     <col min="2" max="2" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="15.139" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="17.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="18.140625" customWidth="true" style="0"/>
+    <col min="5" max="5" width="29.279" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" customHeight="1" ht="21">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" customHeight="1" ht="15">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" customHeight="1" ht="15.75">
       <c r="A3" s="1" t="s">
@@ -591,7 +573,7 @@
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -608,7 +590,7 @@
       <c r="D4" s="2">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -625,7 +607,7 @@
       <c r="D5" s="2">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -642,7 +624,7 @@
       <c r="D6" s="2">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -659,7 +641,7 @@
       <c r="D7" s="2">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -676,7 +658,7 @@
       <c r="D8" s="2">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -693,7 +675,7 @@
       <c r="D9" s="2">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -710,7 +692,7 @@
       <c r="D10" s="2">
         <v>8</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -727,7 +709,7 @@
       <c r="D11" s="2">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -744,7 +726,7 @@
       <c r="D12" s="2">
         <v>8</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -761,7 +743,7 @@
       <c r="D13" s="2">
         <v>8</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -778,7 +760,7 @@
       <c r="D14" s="2">
         <v>8</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -795,7 +777,7 @@
       <c r="D15" s="2">
         <v>8</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -812,7 +794,7 @@
       <c r="D16" s="2">
         <v>8</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -829,7 +811,7 @@
       <c r="D17" s="2">
         <v>8.38</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -846,8 +828,8 @@
       <c r="D18" s="2">
         <v>8.0</v>
       </c>
-      <c r="E18" t="s">
-        <v>28</v>
+      <c r="E18" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>